<commit_message>
Updated review servlet to give more information
</commit_message>
<xml_diff>
--- a/Signature Key.xlsx
+++ b/Signature Key.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\mismo\mismo-trainer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3BAD73-2D81-4EA9-A6E3-9C8CE5C1F56E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8625FECE-1510-4347-AE91-ED442910DD65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="86280" yWindow="-15990" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EF2050D1-8970-4FAD-928E-AE9970E8F71F}"/>
+    <workbookView xWindow="86280" yWindow="-15990" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EF2050D1-8970-4FAD-928E-AE9970E8F71F}"/>
   </bookViews>
   <sheets>
     <sheet name="Keys" sheetId="1" r:id="rId1"/>
     <sheet name="Step Through" sheetId="2" r:id="rId2"/>
+    <sheet name="Output" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Output!$A$1:$G$4</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -59,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="174">
   <si>
     <t>A</t>
   </si>
@@ -557,6 +561,30 @@
   </si>
   <si>
     <t>Signature</t>
+  </si>
+  <si>
+    <t>Patient A ID</t>
+  </si>
+  <si>
+    <t>Patient B ID</t>
+  </si>
+  <si>
+    <t>AITy+4:Qo7iao:Qo7iao:QIbiao</t>
+  </si>
+  <si>
+    <t>AITy+4:Qo7iao:Qo7iao:AIbiao</t>
+  </si>
+  <si>
+    <t>AITy+4</t>
+  </si>
+  <si>
+    <t>Qo7iao</t>
+  </si>
+  <si>
+    <t>QIbiao</t>
+  </si>
+  <si>
+    <t>AIbiao</t>
   </si>
 </sst>
 </file>
@@ -580,7 +608,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -626,6 +654,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -679,7 +713,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -740,6 +774,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1079,7 +1119,7 @@
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A64" sqref="A1:A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2120,18 +2160,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719256B6-3BE1-4CD7-9D03-0A04BB444E0C}">
-  <dimension ref="A1:AK38"/>
+  <dimension ref="A1:AI56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" style="2" hidden="1" customWidth="1"/>
     <col min="6" max="10" width="3.28515625" style="2" customWidth="1"/>
     <col min="11" max="11" width="3.5703125" customWidth="1"/>
     <col min="12" max="15" width="3.85546875" style="2" customWidth="1"/>
@@ -2139,16 +2180,15 @@
     <col min="18" max="18" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="6.7109375" style="2" customWidth="1"/>
-    <col min="24" max="24" width="35.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="29" width="3.28515625" style="2" customWidth="1"/>
-    <col min="30" max="30" width="3.5703125" customWidth="1"/>
-    <col min="31" max="34" width="3.85546875" style="2" customWidth="1"/>
-    <col min="36" max="36" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" style="2" customWidth="1"/>
+    <col min="23" max="27" width="3.28515625" style="2" customWidth="1"/>
+    <col min="28" max="28" width="3.5703125" customWidth="1"/>
+    <col min="29" max="32" width="3.85546875" style="2" customWidth="1"/>
+    <col min="34" max="34" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="35.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E1" s="12" t="s">
         <v>163</v>
       </c>
@@ -2167,26 +2207,23 @@
       <c r="R1" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="X1" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="Z1" s="22" t="s">
+      <c r="X1" s="22" t="s">
         <v>91</v>
       </c>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
       <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
-      <c r="AE1" s="23" t="s">
+      <c r="AC1" s="23" t="s">
         <v>164</v>
       </c>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="23"/>
       <c r="AF1" s="23"/>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AK1" s="19" t="s">
+      <c r="AI1" s="19" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>58</v>
       </c>
@@ -2241,44 +2278,37 @@
       <c r="V2" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="W2" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="X2" s="21" t="str">
-        <f>_xlfn.CONCAT(W3:W36)</f>
-        <v>06000060F0006F70FFF800F08FF8F0F8F0</v>
-      </c>
-      <c r="Y2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y2" s="13" t="s">
+        <v>62</v>
+      </c>
       <c r="Z2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA2" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC2" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="AA2" s="13" t="s">
+      <c r="AD2" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="AB2" s="13" t="s">
+      <c r="AE2" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="AC2" s="13" t="s">
+      <c r="AF2" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="AE2" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF2" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG2" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH2" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="AK2" s="20" t="str">
-        <f>AK3&amp;":"&amp;AK4&amp;":"&amp;AK5&amp;":"&amp;AK6</f>
+      <c r="AI2" s="20" t="str">
+        <f>AI3&amp;":"&amp;AI4&amp;":"&amp;AI5&amp;":"&amp;AI6</f>
         <v>AITy+4:Qo7iao:Qo7iao:AIbiao</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2343,59 +2373,55 @@
         <f>INT(U3*15)</f>
         <v>0</v>
       </c>
-      <c r="W3" s="4" t="str">
-        <f>DEC2HEX(V3)</f>
-        <v>0</v>
-      </c>
-      <c r="Y3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="14">
+        <f>MOD(INT($C3/8),2)</f>
+        <v>0</v>
+      </c>
+      <c r="Y3" s="14">
+        <f>MOD(INT($C3/4),2)</f>
+        <v>0</v>
+      </c>
       <c r="Z3" s="14">
-        <f>MOD(INT($C3/8),2)</f>
+        <f>MOD(INT($C3/2),2)</f>
         <v>0</v>
       </c>
       <c r="AA3" s="14">
-        <f>MOD(INT($C3/4),2)</f>
-        <v>0</v>
-      </c>
-      <c r="AB3" s="14">
-        <f>MOD(INT($C3/2),2)</f>
-        <v>0</v>
-      </c>
-      <c r="AC3" s="14">
         <f>MOD(V3,2)</f>
         <v>0</v>
+      </c>
+      <c r="AC3" s="18" t="str" cm="1">
+        <f t="array" ref="AC3">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(X3:X8))+1)</f>
+        <v>A</v>
+      </c>
+      <c r="AD3" s="18" t="str" cm="1">
+        <f t="array" ref="AD3">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(Y3:Y8))+1)</f>
+        <v>Q</v>
       </c>
       <c r="AE3" s="18" t="str" cm="1">
         <f t="array" ref="AE3">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(Z3:Z8))+1)</f>
-        <v>A</v>
+        <v>Q</v>
       </c>
       <c r="AF3" s="18" t="str" cm="1">
         <f t="array" ref="AF3">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AA3:AA8))+1)</f>
-        <v>Q</v>
-      </c>
-      <c r="AG3" s="18" t="str" cm="1">
-        <f t="array" ref="AG3">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AB3:AB8))+1)</f>
-        <v>Q</v>
-      </c>
-      <c r="AH3" s="18" t="str" cm="1">
-        <f t="array" ref="AH3">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AC3:AC8))+1)</f>
         <v>A</v>
       </c>
-      <c r="AJ3" s="17" t="s">
+      <c r="AH3" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="AK3" s="18" t="str">
-        <f>_xlfn.CONCAT(AE3:AE38)</f>
+      <c r="AI3" s="18" t="str">
+        <f>_xlfn.CONCAT(AC3:AC38)</f>
         <v>AITy+4</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="25">
         <v>0.47</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="24">
         <f t="shared" ref="C4:C36" si="0">INT(B4*15)</f>
         <v>7</v>
       </c>
@@ -2431,44 +2457,39 @@
       <c r="T4" t="s">
         <v>33</v>
       </c>
-      <c r="U4" s="3">
+      <c r="U4" s="25">
         <v>0.44</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V4" s="24">
         <f t="shared" ref="V4:V36" si="6">INT(U4*15)</f>
         <v>6</v>
       </c>
-      <c r="W4" s="4" t="str">
-        <f t="shared" ref="W4:W36" si="7">DEC2HEX(V4)</f>
-        <v>6</v>
-      </c>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="15">
+        <f t="shared" ref="X4:X36" si="7">MOD(INT($C4/8),2)</f>
+        <v>0</v>
+      </c>
+      <c r="Y4" s="15">
+        <f t="shared" ref="Y4:Y36" si="8">MOD(INT($C4/4),2)</f>
+        <v>1</v>
+      </c>
       <c r="Z4" s="15">
-        <f t="shared" ref="Z4:Z36" si="8">MOD(INT($C4/8),2)</f>
-        <v>0</v>
+        <f t="shared" ref="Z4:Z36" si="9">MOD(INT($C4/2),2)</f>
+        <v>1</v>
       </c>
       <c r="AA4" s="15">
-        <f t="shared" ref="AA4:AA36" si="9">MOD(INT($C4/4),2)</f>
-        <v>1</v>
-      </c>
-      <c r="AB4" s="15">
-        <f t="shared" ref="AB4:AB36" si="10">MOD(INT($C4/2),2)</f>
-        <v>1</v>
-      </c>
-      <c r="AC4" s="15">
-        <f t="shared" ref="AC4:AC36" si="11">MOD(V4,2)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="17" t="s">
+        <f>MOD(V4,2)</f>
+        <v>0</v>
+      </c>
+      <c r="AH4" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="AK4" s="18" t="str">
-        <f>_xlfn.CONCAT(AF3:AF38)</f>
+      <c r="AI4" s="18" t="str">
+        <f>_xlfn.CONCAT(AD3:AD38)</f>
         <v>Qo7iao</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -2518,37 +2539,32 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W5" s="4" t="str">
+      <c r="W5" s="4"/>
+      <c r="X5" s="15">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
+      <c r="Y5" s="15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z5" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA5" s="15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB5" s="15">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC5" s="15">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="17" t="s">
+        <f>MOD(V5,2)</f>
+        <v>0</v>
+      </c>
+      <c r="AH5" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="AK5" s="18" t="str">
-        <f>_xlfn.CONCAT(AG3:AG38)</f>
+      <c r="AI5" s="18" t="str">
+        <f>_xlfn.CONCAT(AE3:AE38)</f>
         <v>Qo7iao</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -2598,37 +2614,32 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W6" s="4" t="str">
+      <c r="W6" s="4"/>
+      <c r="X6" s="15">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
+      <c r="Y6" s="15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z6" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA6" s="15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB6" s="15">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC6" s="15">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AJ6" s="17" t="s">
+        <f>MOD(V6,2)</f>
+        <v>0</v>
+      </c>
+      <c r="AH6" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="AK6" s="18" t="str">
-        <f>_xlfn.CONCAT(AH3:AH38)</f>
+      <c r="AI6" s="18" t="str">
+        <f>_xlfn.CONCAT(AF3:AF38)</f>
         <v>AIbiao</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -2671,30 +2682,25 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W7" s="4" t="str">
+      <c r="W7" s="4"/>
+      <c r="X7" s="15">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="4"/>
+      <c r="Y7" s="15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z7" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA7" s="15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB7" s="15">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC7" s="15">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+        <f>MOD(V7,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2737,30 +2743,25 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W8" s="4" t="str">
+      <c r="W8" s="4"/>
+      <c r="X8" s="16">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
+      <c r="Y8" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z8" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA8" s="16">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB8" s="16">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC8" s="16">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+        <f>MOD(V8,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -2819,46 +2820,41 @@
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="W9" s="4" t="str">
+      <c r="W9" s="4"/>
+      <c r="X9" s="5">
         <f t="shared" si="7"/>
-        <v>6</v>
-      </c>
-      <c r="X9" s="4"/>
-      <c r="Y9" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y9" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
       <c r="Z9" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>1</v>
       </c>
       <c r="AA9" s="5">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AB9" s="5">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AC9" s="5">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>MOD(V9,2)</f>
+        <v>0</v>
+      </c>
+      <c r="AC9" s="18" t="str" cm="1">
+        <f t="array" ref="AC9">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(X9:X14))+1)</f>
+        <v>I</v>
+      </c>
+      <c r="AD9" s="18" t="str" cm="1">
+        <f t="array" ref="AD9">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(Y9:Y14))+1)</f>
+        <v>o</v>
       </c>
       <c r="AE9" s="18" t="str" cm="1">
         <f t="array" ref="AE9">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(Z9:Z14))+1)</f>
-        <v>I</v>
+        <v>o</v>
       </c>
       <c r="AF9" s="18" t="str" cm="1">
         <f t="array" ref="AF9">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AA9:AA14))+1)</f>
-        <v>o</v>
-      </c>
-      <c r="AG9" s="18" t="str" cm="1">
-        <f t="array" ref="AG9">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AB9:AB14))+1)</f>
-        <v>o</v>
-      </c>
-      <c r="AH9" s="18" t="str" cm="1">
-        <f t="array" ref="AH9">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AC9:AC14))+1)</f>
         <v>I</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -2901,30 +2897,25 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W10" s="4" t="str">
+      <c r="W10" s="4"/>
+      <c r="X10" s="6">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="4"/>
+      <c r="Y10" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z10" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA10" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB10" s="6">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC10" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+        <f>MOD(V10,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -2967,30 +2958,25 @@
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="W11" s="4" t="str">
+      <c r="W11" s="4"/>
+      <c r="X11" s="6">
         <f t="shared" si="7"/>
-        <v>F</v>
-      </c>
-      <c r="X11" s="4"/>
-      <c r="Y11" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y11" s="6">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
       <c r="Z11" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AA11" s="6">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AB11" s="6">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AC11" s="6">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+        <f>MOD(V11,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -3033,30 +3019,25 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W12" s="4" t="str">
+      <c r="W12" s="4"/>
+      <c r="X12" s="6">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="4"/>
+      <c r="Y12" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z12" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA12" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB12" s="6">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC12" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+        <f>MOD(V12,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -3099,30 +3080,25 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W13" s="4" t="str">
+      <c r="W13" s="4"/>
+      <c r="X13" s="6">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X13" s="4"/>
-      <c r="Y13" s="4"/>
+      <c r="Y13" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z13" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA13" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB13" s="6">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC13" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+        <f>MOD(V13,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -3165,30 +3141,25 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W14" s="4" t="str">
+      <c r="W14" s="4"/>
+      <c r="X14" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
+      <c r="Y14" s="7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z14" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA14" s="7">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB14" s="7">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC14" s="7">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+        <f>MOD(V14,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -3247,46 +3218,41 @@
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="W15" s="4" t="str">
+      <c r="W15" s="4"/>
+      <c r="X15" s="14">
         <f t="shared" si="7"/>
-        <v>6</v>
-      </c>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y15" s="14">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
       <c r="Z15" s="14">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>1</v>
       </c>
       <c r="AA15" s="14">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AB15" s="14">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AC15" s="14">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>MOD(V15,2)</f>
+        <v>0</v>
+      </c>
+      <c r="AC15" s="18" t="str" cm="1">
+        <f t="array" ref="AC15">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(X15:X20))+1)</f>
+        <v>T</v>
+      </c>
+      <c r="AD15" s="18" t="str" cm="1">
+        <f t="array" ref="AD15">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(Y15:Y20))+1)</f>
+        <v>7</v>
       </c>
       <c r="AE15" s="18" t="str" cm="1">
         <f t="array" ref="AE15">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(Z15:Z20))+1)</f>
-        <v>T</v>
+        <v>7</v>
       </c>
       <c r="AF15" s="18" t="str" cm="1">
         <f t="array" ref="AF15">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AA15:AA20))+1)</f>
-        <v>7</v>
-      </c>
-      <c r="AG15" s="18" t="str" cm="1">
-        <f t="array" ref="AG15">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AB15:AB20))+1)</f>
-        <v>7</v>
-      </c>
-      <c r="AH15" s="18" t="str" cm="1">
-        <f t="array" ref="AH15">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AC15:AC20))+1)</f>
         <v>b</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -3329,30 +3295,25 @@
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="W16" s="4" t="str">
+      <c r="W16" s="4"/>
+      <c r="X16" s="15">
         <f t="shared" si="7"/>
-        <v>F</v>
-      </c>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y16" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
       <c r="Z16" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AA16" s="15">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AB16" s="15">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AC16" s="15">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V16,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -3395,30 +3356,25 @@
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="W17" s="4" t="str">
+      <c r="W17" s="4"/>
+      <c r="X17" s="15">
         <f t="shared" si="7"/>
-        <v>7</v>
-      </c>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y17" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
       <c r="Z17" s="15">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>1</v>
       </c>
       <c r="AA17" s="15">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AB17" s="15">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AC17" s="15">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V17,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -3461,30 +3417,25 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W18" s="4" t="str">
+      <c r="W18" s="4"/>
+      <c r="X18" s="15">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
+      <c r="Y18" s="15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z18" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA18" s="15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB18" s="15">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC18" s="15">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V18,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -3527,30 +3478,25 @@
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="W19" s="4" t="str">
+      <c r="W19" s="4"/>
+      <c r="X19" s="15">
         <f t="shared" si="7"/>
-        <v>F</v>
-      </c>
-      <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y19" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
       <c r="Z19" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AA19" s="15">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AB19" s="15">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AC19" s="15">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V19,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -3593,30 +3539,25 @@
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="W20" s="4" t="str">
+      <c r="W20" s="4"/>
+      <c r="X20" s="16">
         <f t="shared" si="7"/>
-        <v>F</v>
-      </c>
-      <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y20" s="16">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
       <c r="Z20" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AA20" s="16">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AB20" s="16">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AC20" s="16">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V20,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -3675,46 +3616,41 @@
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="W21" s="4" t="str">
+      <c r="W21" s="4"/>
+      <c r="X21" s="5">
         <f t="shared" si="7"/>
-        <v>F</v>
-      </c>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y21" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
       <c r="Z21" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AA21" s="5">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AB21" s="5">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AC21" s="5">
-        <f t="shared" si="11"/>
-        <v>1</v>
+        <f>MOD(V21,2)</f>
+        <v>1</v>
+      </c>
+      <c r="AC21" s="18" t="str" cm="1">
+        <f t="array" ref="AC21">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(X21:X26))+1)</f>
+        <v>y</v>
+      </c>
+      <c r="AD21" s="18" t="str" cm="1">
+        <f t="array" ref="AD21">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(Y21:Y26))+1)</f>
+        <v>i</v>
       </c>
       <c r="AE21" s="18" t="str" cm="1">
         <f t="array" ref="AE21">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(Z21:Z26))+1)</f>
-        <v>y</v>
+        <v>i</v>
       </c>
       <c r="AF21" s="18" t="str" cm="1">
         <f t="array" ref="AF21">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AA21:AA26))+1)</f>
         <v>i</v>
       </c>
-      <c r="AG21" s="18" t="str" cm="1">
-        <f t="array" ref="AG21">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AB21:AB26))+1)</f>
-        <v>i</v>
-      </c>
-      <c r="AH21" s="18" t="str" cm="1">
-        <f t="array" ref="AH21">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AC21:AC26))+1)</f>
-        <v>i</v>
-      </c>
-    </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -3757,30 +3693,25 @@
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="W22" s="4" t="str">
+      <c r="W22" s="4"/>
+      <c r="X22" s="6">
         <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="X22" s="4"/>
-      <c r="Y22" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y22" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z22" s="6">
-        <f t="shared" si="8"/>
-        <v>1</v>
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="AA22" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB22" s="6">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC22" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V22,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -3823,30 +3754,25 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W23" s="4" t="str">
+      <c r="W23" s="4"/>
+      <c r="X23" s="6">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X23" s="4"/>
-      <c r="Y23" s="4"/>
+      <c r="Y23" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z23" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA23" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB23" s="6">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC23" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V23,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -3889,30 +3815,25 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W24" s="4" t="str">
+      <c r="W24" s="4"/>
+      <c r="X24" s="6">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
+      <c r="Y24" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z24" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA24" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB24" s="6">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC24" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V24,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -3955,30 +3876,25 @@
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="W25" s="4" t="str">
+      <c r="W25" s="4"/>
+      <c r="X25" s="6">
         <f t="shared" si="7"/>
-        <v>F</v>
-      </c>
-      <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y25" s="6">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
       <c r="Z25" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AA25" s="6">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AB25" s="6">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AC25" s="6">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V25,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -4021,30 +3937,25 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W26" s="4" t="str">
+      <c r="W26" s="4"/>
+      <c r="X26" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
+      <c r="Y26" s="7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z26" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA26" s="7">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB26" s="7">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC26" s="7">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V26,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -4103,46 +4014,41 @@
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="W27" s="4" t="str">
+      <c r="W27" s="4"/>
+      <c r="X27" s="14">
         <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y27" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z27" s="14">
-        <f t="shared" si="8"/>
-        <v>1</v>
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="AA27" s="14">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB27" s="14">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC27" s="14">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>MOD(V27,2)</f>
+        <v>0</v>
+      </c>
+      <c r="AC27" s="18" t="str" cm="1">
+        <f t="array" ref="AC27">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(X27:X32))+1)</f>
+        <v>+</v>
+      </c>
+      <c r="AD27" s="18" t="str" cm="1">
+        <f t="array" ref="AD27">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(Y27:Y32))+1)</f>
+        <v>a</v>
       </c>
       <c r="AE27" s="18" t="str" cm="1">
         <f t="array" ref="AE27">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(Z27:Z32))+1)</f>
-        <v>+</v>
+        <v>a</v>
       </c>
       <c r="AF27" s="18" t="str" cm="1">
         <f t="array" ref="AF27">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AA27:AA32))+1)</f>
         <v>a</v>
       </c>
-      <c r="AG27" s="18" t="str" cm="1">
-        <f t="array" ref="AG27">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AB27:AB32))+1)</f>
-        <v>a</v>
-      </c>
-      <c r="AH27" s="18" t="str" cm="1">
-        <f t="array" ref="AH27">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AC27:AC32))+1)</f>
-        <v>a</v>
-      </c>
-    </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -4185,30 +4091,25 @@
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="W28" s="4" t="str">
+      <c r="W28" s="4"/>
+      <c r="X28" s="15">
         <f t="shared" si="7"/>
-        <v>F</v>
-      </c>
-      <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y28" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
       <c r="Z28" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AA28" s="15">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AB28" s="15">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AC28" s="15">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V28,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -4251,30 +4152,25 @@
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="W29" s="4" t="str">
+      <c r="W29" s="4"/>
+      <c r="X29" s="15">
         <f t="shared" si="7"/>
-        <v>F</v>
-      </c>
-      <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y29" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
       <c r="Z29" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AA29" s="15">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AB29" s="15">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AC29" s="15">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V29,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>51</v>
       </c>
@@ -4317,30 +4213,25 @@
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="W30" s="4" t="str">
+      <c r="W30" s="4"/>
+      <c r="X30" s="15">
         <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="X30" s="4"/>
-      <c r="Y30" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y30" s="15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z30" s="15">
-        <f t="shared" si="8"/>
-        <v>1</v>
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="AA30" s="15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB30" s="15">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC30" s="15">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V30,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -4383,30 +4274,25 @@
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="W31" s="4" t="str">
+      <c r="W31" s="4"/>
+      <c r="X31" s="15">
         <f t="shared" si="7"/>
-        <v>F</v>
-      </c>
-      <c r="X31" s="4"/>
-      <c r="Y31" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y31" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
       <c r="Z31" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AA31" s="15">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AB31" s="15">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AC31" s="15">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V31,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -4449,30 +4335,25 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W32" s="4" t="str">
+      <c r="W32" s="4"/>
+      <c r="X32" s="16">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
+      <c r="Y32" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z32" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA32" s="16">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB32" s="16">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC32" s="16">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V32,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -4531,46 +4412,41 @@
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="W33" s="4" t="str">
+      <c r="W33" s="4"/>
+      <c r="X33" s="5">
         <f t="shared" si="7"/>
-        <v>F</v>
-      </c>
-      <c r="X33" s="4"/>
-      <c r="Y33" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y33" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
       <c r="Z33" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AA33" s="5">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AB33" s="5">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AC33" s="5">
-        <f t="shared" si="11"/>
-        <v>1</v>
+        <f>MOD(V33,2)</f>
+        <v>1</v>
+      </c>
+      <c r="AC33" s="18" t="str" cm="1">
+        <f t="array" ref="AC33">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(X33:X38))+1)</f>
+        <v>4</v>
+      </c>
+      <c r="AD33" s="18" t="str" cm="1">
+        <f t="array" ref="AD33">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(Y33:Y38))+1)</f>
+        <v>o</v>
       </c>
       <c r="AE33" s="18" t="str" cm="1">
         <f t="array" ref="AE33">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(Z33:Z38))+1)</f>
-        <v>4</v>
+        <v>o</v>
       </c>
       <c r="AF33" s="18" t="str" cm="1">
         <f t="array" ref="AF33">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AA33:AA38))+1)</f>
         <v>o</v>
       </c>
-      <c r="AG33" s="18" t="str" cm="1">
-        <f t="array" ref="AG33">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AB33:AB38))+1)</f>
-        <v>o</v>
-      </c>
-      <c r="AH33" s="18" t="str" cm="1">
-        <f t="array" ref="AH33">INDEX(Keys!$A$1:$A$64,BIN2DEC(_xlfn.CONCAT(AC33:AC38))+1)</f>
-        <v>o</v>
-      </c>
-    </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -4613,30 +4489,25 @@
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="W34" s="4" t="str">
+      <c r="W34" s="4"/>
+      <c r="X34" s="6">
         <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="X34" s="4"/>
-      <c r="Y34" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y34" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z34" s="6">
-        <f t="shared" si="8"/>
-        <v>1</v>
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="AA34" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB34" s="6">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC34" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V34,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -4679,30 +4550,25 @@
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="W35" s="4" t="str">
+      <c r="W35" s="4"/>
+      <c r="X35" s="6">
         <f t="shared" si="7"/>
-        <v>F</v>
-      </c>
-      <c r="X35" s="4"/>
-      <c r="Y35" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y35" s="6">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
       <c r="Z35" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AA35" s="6">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AB35" s="6">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AC35" s="6">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V35,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -4745,30 +4611,25 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W36" s="4" t="str">
+      <c r="W36" s="4"/>
+      <c r="X36" s="6">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X36" s="4"/>
-      <c r="Y36" s="4"/>
+      <c r="Y36" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="Z36" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA36" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB36" s="6">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC36" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
+        <f>MOD(V36,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="G37" s="8">
         <v>0</v>
       </c>
@@ -4781,20 +4642,20 @@
       <c r="J37" s="8">
         <v>0</v>
       </c>
+      <c r="X37" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="8">
+        <v>0</v>
+      </c>
       <c r="Z37" s="8">
         <v>0</v>
       </c>
       <c r="AA37" s="8">
         <v>0</v>
       </c>
-      <c r="AB37" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC37" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
       <c r="G38" s="9">
         <v>0</v>
       </c>
@@ -4807,27 +4668,427 @@
       <c r="J38" s="9">
         <v>0</v>
       </c>
+      <c r="X38" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="9">
+        <v>0</v>
+      </c>
       <c r="Z38" s="9">
         <v>0</v>
       </c>
       <c r="AA38" s="9">
         <v>0</v>
       </c>
-      <c r="AB38" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC38" s="9">
-        <v>0</v>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="D41" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="D42" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="D43" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="D44" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="D45" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="D46" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="D47" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="D48" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <v>10</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <v>11</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <v>12</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <v>13</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55" s="2">
+        <v>14</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="2">
+        <v>15</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="L1:O1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AE1:AH1"/>
+    <mergeCell ref="X1:AA1"/>
+    <mergeCell ref="AC1:AF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A201EDF-AF61-4467-B533-76436110E229}">
+  <dimension ref="A1:AO4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G2" t="s">
+        <v>172</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0.47</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0.44</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0.46</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>0.48</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0.54</v>
+      </c>
+      <c r="AG2">
+        <v>1</v>
+      </c>
+      <c r="AH2">
+        <v>1</v>
+      </c>
+      <c r="AI2">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AJ2">
+        <v>1</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>1</v>
+      </c>
+      <c r="AM2">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AN2">
+        <v>1</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>567</v>
+      </c>
+      <c r="B4">
+        <v>765</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G4" xr:uid="{8A201EDF-AF61-4467-B533-76436110E229}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>